<commit_message>
Primeiro protóripo 100% funcional
</commit_message>
<xml_diff>
--- a/dados.xlsx
+++ b/dados.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:E1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -429,7 +429,7 @@
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>Valor</t>
+          <t>Valor aproximado</t>
         </is>
       </c>
       <c r="C1" t="inlineStr">
@@ -442,112 +442,9 @@
           <t>Nome do cliente</t>
         </is>
       </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="n">
-        <v>1</v>
-      </c>
-      <c r="B2" t="n">
-        <v>500</v>
-      </c>
-      <c r="C2" t="inlineStr">
+      <c r="E1" t="inlineStr">
         <is>
-          <t>20/20/2020</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>Jean</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="n">
-        <v>2</v>
-      </c>
-      <c r="B3" t="n">
-        <v>50</v>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>10/10/2022</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>Jean Carlos</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="n">
-        <v>3</v>
-      </c>
-      <c r="B4" t="n">
-        <v>50</v>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>20/30/2021</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>Jean</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="n">
-        <v>4</v>
-      </c>
-      <c r="B5" t="n">
-        <v>100</v>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>20/20/2020</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>Carlos</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="n">
-        <v>5</v>
-      </c>
-      <c r="B6" t="n">
-        <v>2500</v>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>20/20/2020</t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>Jean</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="n">
-        <v>6</v>
-      </c>
-      <c r="B7" t="n">
-        <v>100</v>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>20</t>
-        </is>
-      </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>teste</t>
+          <t>Tipo bolo</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
correção de bug na hora de dar baixa
</commit_message>
<xml_diff>
--- a/dados.xlsx
+++ b/dados.xlsx
@@ -2,15 +2,14 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
-  <workbookProtection/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="20370" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Dados" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
@@ -46,11 +45,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
@@ -413,13 +413,16 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E1"/>
+  <dimension ref="A1:E13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="15" customWidth="1" style="1" min="3" max="3"/>
+  </cols>
   <sheetData>
     <row r="1">
       <c r="A1" t="inlineStr">
@@ -445,6 +448,258 @@
       <c r="E1" t="inlineStr">
         <is>
           <t>Tipo bolo</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" t="n">
+        <v>250</v>
+      </c>
+      <c r="C2" t="n">
+        <v>50</v>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>Jean</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>Aniversário</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" t="n">
+        <v>500</v>
+      </c>
+      <c r="C3" t="n">
+        <v>50</v>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>NAejc</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>Casamento</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" t="n">
+        <v>750</v>
+      </c>
+      <c r="C4" t="n">
+        <v>50</v>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>Jean</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>Casamento</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>4</v>
+      </c>
+      <c r="B5" t="n">
+        <v>1000</v>
+      </c>
+      <c r="C5" t="n">
+        <v>50</v>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>NAejc</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>Casamento</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>5</v>
+      </c>
+      <c r="B6" t="n">
+        <v>1250</v>
+      </c>
+      <c r="C6" t="n">
+        <v>50</v>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>Jean</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>Aniversário</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>6</v>
+      </c>
+      <c r="B7" t="n">
+        <v>1500</v>
+      </c>
+      <c r="C7" t="n">
+        <v>50</v>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>NAejc</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>Casamento</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>7</v>
+      </c>
+      <c r="B8" t="n">
+        <v>1750</v>
+      </c>
+      <c r="C8" t="n">
+        <v>50</v>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>Jean</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>Aniversário</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>8</v>
+      </c>
+      <c r="B9" t="n">
+        <v>2000</v>
+      </c>
+      <c r="C9" t="n">
+        <v>50</v>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>NAejc</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>Casamento</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>9</v>
+      </c>
+      <c r="B10" t="n">
+        <v>2250</v>
+      </c>
+      <c r="C10" t="n">
+        <v>50</v>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>Jean</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>Aniversário</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>10</v>
+      </c>
+      <c r="B11" t="n">
+        <v>2500</v>
+      </c>
+      <c r="C11" t="n">
+        <v>50</v>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>NAejc</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>Casamento</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>11</v>
+      </c>
+      <c r="B12" t="n">
+        <v>2750</v>
+      </c>
+      <c r="C12" t="n">
+        <v>50</v>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>Jean</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>Aniversário</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="n">
+        <v>12</v>
+      </c>
+      <c r="B13" t="n">
+        <v>3250</v>
+      </c>
+      <c r="C13" t="n">
+        <v>50</v>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>Jean</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>Aniversário</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Nova versão do menu
</commit_message>
<xml_diff>
--- a/dados.xlsx
+++ b/dados.xlsx
@@ -412,7 +412,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I5"/>
+  <dimension ref="A1:I8"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="H3" sqref="H3"/>
@@ -613,6 +613,102 @@
         </is>
       </c>
     </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>5</v>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Jean</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>20</t>
+        </is>
+      </c>
+      <c r="D6" t="n">
+        <v>20</v>
+      </c>
+      <c r="E6" t="n">
+        <v>20</v>
+      </c>
+      <c r="F6" t="n">
+        <v>20</v>
+      </c>
+      <c r="G6" t="n">
+        <v>20</v>
+      </c>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t>Pendente</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>6</v>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Jean</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>202020</t>
+        </is>
+      </c>
+      <c r="D7" t="n">
+        <v>20</v>
+      </c>
+      <c r="E7" t="n">
+        <v>20</v>
+      </c>
+      <c r="F7" t="n">
+        <v>20</v>
+      </c>
+      <c r="G7" t="n">
+        <v>20</v>
+      </c>
+      <c r="I7" t="inlineStr">
+        <is>
+          <t>Pendente</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>7</v>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Jean</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>20</t>
+        </is>
+      </c>
+      <c r="D8" t="n">
+        <v>20</v>
+      </c>
+      <c r="E8" t="n">
+        <v>20</v>
+      </c>
+      <c r="F8" t="n">
+        <v>20</v>
+      </c>
+      <c r="G8" t="n">
+        <v>2</v>
+      </c>
+      <c r="I8" t="inlineStr">
+        <is>
+          <t>Pendente</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
MENU DE LISTAGEM CONCLUIDO
</commit_message>
<xml_diff>
--- a/dados.xlsx
+++ b/dados.xlsx
@@ -484,12 +484,12 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Jean</t>
+          <t>Jean Carlos</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>20/10/2021</t>
+          <t>01/01/2021</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -508,19 +508,6 @@
       </c>
       <c r="H2" t="n">
         <v>4</v>
-      </c>
-      <c r="J2" t="inlineStr">
-        <is>
-          <t>1
-2
-3
-4
-5
-6
-7
-8
-Teste</t>
-        </is>
       </c>
       <c r="K2" t="inlineStr">
         <is>
@@ -534,21 +521,21 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Jean</t>
+          <t xml:space="preserve">Carlos </t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>20</t>
+          <t>02/02/2021</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>20</t>
+          <t>10:45</t>
         </is>
       </c>
       <c r="E3" t="n">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="F3" t="n">
         <v>20</v>
@@ -558,11 +545,6 @@
       </c>
       <c r="H3" t="n">
         <v>20</v>
-      </c>
-      <c r="J3" t="inlineStr">
-        <is>
-          <t>Jean Carlos</t>
-        </is>
       </c>
       <c r="K3" t="inlineStr">
         <is>
@@ -576,37 +558,32 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>20</t>
+          <t>Naejc</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>20</t>
+          <t>01/01/2021</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>20</t>
+          <t>10:45</t>
         </is>
       </c>
       <c r="E4" t="n">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="F4" t="n">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="G4" t="n">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="H4" t="n">
-        <v>20</v>
-      </c>
-      <c r="J4" t="inlineStr">
-        <is>
-          <t>Jean Carlos
-20</t>
-        </is>
-      </c>
+        <v>10</v>
+      </c>
+      <c r="J4" t="inlineStr"/>
       <c r="K4" t="inlineStr">
         <is>
           <t>Pendente</t>

</xml_diff>

<commit_message>
LISTAR ENCOMENDAS 100% CONCLUÍDO
</commit_message>
<xml_diff>
--- a/dados.xlsx
+++ b/dados.xlsx
@@ -1,34 +1,100 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
   <workbookPr/>
-  <workbookProtection/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jeanc\Desktop\projeto\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA3E9C30-3EFB-41BD-8B0D-BBEA42609AD5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Dados" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Dados" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="19">
+  <si>
+    <t>ID</t>
+  </si>
+  <si>
+    <t>Nome cliente</t>
+  </si>
+  <si>
+    <t>Data de entrega</t>
+  </si>
+  <si>
+    <t>Hora de entrega</t>
+  </si>
+  <si>
+    <t>Bolo de aniversário</t>
+  </si>
+  <si>
+    <t>Bolo de casamento</t>
+  </si>
+  <si>
+    <t>Salgado mini</t>
+  </si>
+  <si>
+    <t>Salgado normal</t>
+  </si>
+  <si>
+    <t>Valor final</t>
+  </si>
+  <si>
+    <t>Mensagem adicional</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>Jean Carlos</t>
+  </si>
+  <si>
+    <t>01/01/2021</t>
+  </si>
+  <si>
+    <t>10:45</t>
+  </si>
+  <si>
+    <t>Pendente</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Carlos </t>
+  </si>
+  <si>
+    <t>02/02/2021</t>
+  </si>
+  <si>
+    <t>Naejc</t>
+  </si>
+  <si>
+    <t>Olá</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <color theme="1"/>
-      <sz val="11"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill/>
+      <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -47,80 +113,21 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008000"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00808000"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="00C0C0C0"/>
-      <rgbColor rgb="00808080"/>
-      <rgbColor rgb="009999FF"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00FFFFCC"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00660066"/>
-      <rgbColor rgb="00FF8080"/>
-      <rgbColor rgb="000066CC"/>
-      <rgbColor rgb="00CCCCFF"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="0000CCFF"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00CCFFCC"/>
-      <rgbColor rgb="00FFFF99"/>
-      <rgbColor rgb="0099CCFF"/>
-      <rgbColor rgb="00FF99CC"/>
-      <rgbColor rgb="00CC99FF"/>
-      <rgbColor rgb="00FFCC99"/>
-      <rgbColor rgb="003366FF"/>
-      <rgbColor rgb="0033CCCC"/>
-      <rgbColor rgb="0099CC00"/>
-      <rgbColor rgb="00FFCC00"/>
-      <rgbColor rgb="00FF9900"/>
-      <rgbColor rgb="00FF6600"/>
-      <rgbColor rgb="00666699"/>
-      <rgbColor rgb="00969696"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
-    </indexedColors>
-  </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -408,186 +415,156 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="13.5703125" customWidth="1"/>
+    <col min="3" max="3" width="18.85546875" customWidth="1"/>
+    <col min="4" max="4" width="12.28515625" customWidth="1"/>
+    <col min="5" max="5" width="20.28515625" customWidth="1"/>
+    <col min="6" max="6" width="19.42578125" customWidth="1"/>
+    <col min="7" max="7" width="19.28515625" customWidth="1"/>
+    <col min="8" max="8" width="11.42578125" customWidth="1"/>
+    <col min="9" max="9" width="12.140625" customWidth="1"/>
+    <col min="10" max="10" width="16" customWidth="1"/>
+    <col min="11" max="11" width="12" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>ID</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>Nome cliente</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>Data de entrega</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>Hora de entrega</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>Bolo de aniversário</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>Bolo de casamento</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>Salgado mini</t>
-        </is>
-      </c>
-      <c r="H1" t="inlineStr">
-        <is>
-          <t>Salgado normal</t>
-        </is>
-      </c>
-      <c r="I1" t="inlineStr">
-        <is>
-          <t>Valor final</t>
-        </is>
-      </c>
-      <c r="J1" t="inlineStr">
-        <is>
-          <t>Mensagem adicional</t>
-        </is>
-      </c>
-      <c r="K1" t="inlineStr">
-        <is>
-          <t>Status</t>
-        </is>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" t="s">
+        <v>10</v>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" t="n">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2">
         <v>1</v>
       </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>Jean Carlos</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>01/01/2021</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>10:45</t>
-        </is>
-      </c>
-      <c r="E2" t="n">
+      <c r="B2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2">
         <v>1</v>
       </c>
-      <c r="F2" t="n">
+      <c r="F2">
         <v>2</v>
       </c>
-      <c r="G2" t="n">
+      <c r="G2">
         <v>3</v>
       </c>
-      <c r="H2" t="n">
+      <c r="H2">
         <v>4</v>
       </c>
-      <c r="K2" t="inlineStr">
-        <is>
-          <t>Pendente</t>
-        </is>
+      <c r="J2" t="s">
+        <v>18</v>
+      </c>
+      <c r="K2" t="s">
+        <v>14</v>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" t="n">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3">
         <v>2</v>
       </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Carlos </t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>02/02/2021</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>10:45</t>
-        </is>
-      </c>
-      <c r="E3" t="n">
+      <c r="B3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E3">
         <v>10</v>
       </c>
-      <c r="F3" t="n">
+      <c r="F3">
         <v>20</v>
       </c>
-      <c r="G3" t="n">
+      <c r="G3">
         <v>20</v>
       </c>
-      <c r="H3" t="n">
+      <c r="H3">
         <v>20</v>
       </c>
-      <c r="K3" t="inlineStr">
-        <is>
-          <t>Pendente</t>
-        </is>
+      <c r="J3" t="s">
+        <v>18</v>
+      </c>
+      <c r="K3" t="s">
+        <v>14</v>
       </c>
     </row>
-    <row r="4">
-      <c r="A4" t="n">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4">
         <v>3</v>
       </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>Naejc</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>01/01/2021</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>10:45</t>
-        </is>
-      </c>
-      <c r="E4" t="n">
+      <c r="B4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E4">
         <v>10</v>
       </c>
-      <c r="F4" t="n">
+      <c r="F4">
         <v>10</v>
       </c>
-      <c r="G4" t="n">
+      <c r="G4">
         <v>10</v>
       </c>
-      <c r="H4" t="n">
+      <c r="H4">
         <v>10</v>
       </c>
-      <c r="J4" t="inlineStr"/>
-      <c r="K4" t="inlineStr">
-        <is>
-          <t>Pendente</t>
-        </is>
+      <c r="J4" t="s">
+        <v>18</v>
+      </c>
+      <c r="K4" t="s">
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Att(Ainda falta corrigir bug na janela de popup)
</commit_message>
<xml_diff>
--- a/dados.xlsx
+++ b/dados.xlsx
@@ -1,12 +1,12 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Dados" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Dados" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="0" fullCalcOnLoad="1"/>
@@ -412,7 +412,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K7"/>
+  <dimension ref="A1:K8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="G6" sqref="G6"/>
@@ -723,8 +723,6 @@
       <c r="A7" t="n">
         <v>6</v>
       </c>
-      <c r="B7" t="inlineStr"/>
-      <c r="C7" t="inlineStr"/>
       <c r="D7" t="inlineStr">
         <is>
           <t>00:00</t>
@@ -751,6 +749,48 @@
         </is>
       </c>
       <c r="K7" t="inlineStr">
+        <is>
+          <t>Pendente</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>7</v>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Vinicius</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>09/04/2022</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>01:00</t>
+        </is>
+      </c>
+      <c r="E8" t="n">
+        <v>1000</v>
+      </c>
+      <c r="F8" t="n">
+        <v>0</v>
+      </c>
+      <c r="G8" t="n">
+        <v>300</v>
+      </c>
+      <c r="H8" t="n">
+        <v>14000</v>
+      </c>
+      <c r="J8" t="inlineStr">
+        <is>
+          <t>90000 kg</t>
+        </is>
+      </c>
+      <c r="K8" t="inlineStr">
         <is>
           <t>Pendente</t>
         </is>

</xml_diff>

<commit_message>
Módulo de finalização de pedido concluído
</commit_message>
<xml_diff>
--- a/dados.xlsx
+++ b/dados.xlsx
@@ -412,10 +412,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K8"/>
+  <dimension ref="A1:K12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J13" sqref="J13"/>
+      <selection activeCell="A9" sqref="A9:XFD9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
@@ -563,12 +563,15 @@
       <c r="H3" t="n">
         <v>20</v>
       </c>
+      <c r="I3" t="n">
+        <v>772</v>
+      </c>
       <c r="J3" t="n">
         <v>2</v>
       </c>
       <c r="K3" t="inlineStr">
         <is>
-          <t>Pendente</t>
+          <t>Concluído</t>
         </is>
       </c>
     </row>
@@ -603,12 +606,15 @@
       <c r="H4" t="n">
         <v>10</v>
       </c>
+      <c r="I4" t="n">
+        <v>761</v>
+      </c>
       <c r="J4" t="n">
         <v>3</v>
       </c>
       <c r="K4" t="inlineStr">
         <is>
-          <t>Pendente</t>
+          <t>Concluído</t>
         </is>
       </c>
     </row>
@@ -643,12 +649,15 @@
       <c r="H5" t="n">
         <v>1</v>
       </c>
+      <c r="I5" t="n">
+        <v>751.45</v>
+      </c>
       <c r="J5" t="n">
         <v>4</v>
       </c>
       <c r="K5" t="inlineStr">
         <is>
-          <t>Pendente</t>
+          <t>Concluído</t>
         </is>
       </c>
     </row>
@@ -683,12 +692,15 @@
       <c r="H6" t="n">
         <v>15</v>
       </c>
+      <c r="I6" t="n">
+        <v>766.5</v>
+      </c>
       <c r="J6" t="n">
         <v>5</v>
       </c>
       <c r="K6" t="inlineStr">
         <is>
-          <t>Pendente</t>
+          <t>Concluído</t>
         </is>
       </c>
     </row>
@@ -713,12 +725,15 @@
       <c r="H7" t="n">
         <v>0</v>
       </c>
+      <c r="I7" t="n">
+        <v>75750</v>
+      </c>
       <c r="J7" t="n">
         <v>6</v>
       </c>
       <c r="K7" t="inlineStr">
         <is>
-          <t>Pendente</t>
+          <t>Concluído</t>
         </is>
       </c>
     </row>
@@ -754,12 +769,182 @@
         <v>14000</v>
       </c>
       <c r="I8" t="n">
-        <v>10755</v>
+        <v>11355</v>
       </c>
       <c r="J8" t="n">
         <v>7</v>
       </c>
       <c r="K8" t="inlineStr">
+        <is>
+          <t>Concluído</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>8</v>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>fasdfasdf</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>asdfasdf</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>00:00</t>
+        </is>
+      </c>
+      <c r="E9" t="n">
+        <v>50</v>
+      </c>
+      <c r="F9" t="n">
+        <v>50</v>
+      </c>
+      <c r="G9" t="n">
+        <v>50</v>
+      </c>
+      <c r="H9" t="n">
+        <v>50</v>
+      </c>
+      <c r="I9" t="n">
+        <v>7575757555</v>
+      </c>
+      <c r="J9" t="inlineStr">
+        <is>
+          <t>dvasdfasdfasdfasdfasdfs</t>
+        </is>
+      </c>
+      <c r="K9" t="inlineStr">
+        <is>
+          <t>Concluído</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>9</v>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>sadfasdfasd</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>20</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>20</t>
+        </is>
+      </c>
+      <c r="E10" t="n">
+        <v>20</v>
+      </c>
+      <c r="F10" t="n">
+        <v>202</v>
+      </c>
+      <c r="G10" t="n">
+        <v>2</v>
+      </c>
+      <c r="H10" t="n">
+        <v>2</v>
+      </c>
+      <c r="I10" t="n">
+        <v>21212102.2</v>
+      </c>
+      <c r="J10" t="inlineStr">
+        <is>
+          <t>02	02	02	02	02	02	02	0</t>
+        </is>
+      </c>
+      <c r="K10" t="inlineStr">
+        <is>
+          <t>Concluído</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>10</v>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>asdasdasds</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>dasdasdasd</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>20</t>
+        </is>
+      </c>
+      <c r="E11" t="n">
+        <v>2</v>
+      </c>
+      <c r="F11" t="n">
+        <v>2</v>
+      </c>
+      <c r="G11" t="n">
+        <v>2</v>
+      </c>
+      <c r="H11" t="n">
+        <v>20</v>
+      </c>
+      <c r="I11" t="n">
+        <v>315.7</v>
+      </c>
+      <c r="K11" t="inlineStr">
+        <is>
+          <t>Concluído</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>11</v>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>asdfasdfasdf</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>fasdfasdf</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>20</t>
+        </is>
+      </c>
+      <c r="E12" t="n">
+        <v>20</v>
+      </c>
+      <c r="F12" t="n">
+        <v>20</v>
+      </c>
+      <c r="G12" t="n">
+        <v>20</v>
+      </c>
+      <c r="H12" t="n">
+        <v>20</v>
+      </c>
+      <c r="I12" t="n">
+        <v>322</v>
+      </c>
+      <c r="K12" t="inlineStr">
         <is>
           <t>Concluído</t>
         </is>

</xml_diff>

<commit_message>
Otimizações feitas no SETUP
</commit_message>
<xml_diff>
--- a/dados.xlsx
+++ b/dados.xlsx
@@ -412,7 +412,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K14"/>
+  <dimension ref="A1:K15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A9" sqref="A9:XFD9"/>
@@ -1035,6 +1035,46 @@
         </is>
       </c>
     </row>
+    <row r="15">
+      <c r="A15" t="n">
+        <v>14</v>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>Jean</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>20</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>20</t>
+        </is>
+      </c>
+      <c r="E15" t="n">
+        <v>0</v>
+      </c>
+      <c r="F15" t="n">
+        <v>20</v>
+      </c>
+      <c r="G15" t="n">
+        <v>20</v>
+      </c>
+      <c r="H15" t="n">
+        <v>20</v>
+      </c>
+      <c r="I15" t="n">
+        <v>772</v>
+      </c>
+      <c r="K15" t="inlineStr">
+        <is>
+          <t>Concluído</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Teste no troço lá
</commit_message>
<xml_diff>
--- a/dados.xlsx
+++ b/dados.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rodrigues\Desktop\projeto\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jeanc\Desktop\Projeto\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6460C5D-F322-427B-9DA0-BCB4EE71E782}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B8E8ACC-4BA8-4D6B-A63C-DD613937398E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="20370" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Dados" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="30">
   <si>
     <t>ID</t>
   </si>
@@ -98,16 +98,50 @@
   </si>
   <si>
     <t>alimento</t>
+  </si>
+  <si>
+    <t>JEAN CARLOS</t>
+  </si>
+  <si>
+    <t>20/12/2022</t>
+  </si>
+  <si>
+    <t>TESTE
+TESTE
+TESTE
+TESTE
+TESTE
+TESE
+TESTE
+TESTE
+TESTE
+TEST
+TEST
+TES
+TE
+TEST
+TESTE
+ETSTE
+TETSS</t>
+  </si>
+  <si>
+    <t>01/01/2023</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -133,9 +167,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -438,15 +471,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K5"/>
+  <dimension ref="A1:K6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
@@ -587,8 +620,8 @@
       <c r="B5" t="s">
         <v>24</v>
       </c>
-      <c r="C5" s="1">
-        <v>44562</v>
+      <c r="C5" t="s">
+        <v>29</v>
       </c>
       <c r="D5" t="s">
         <v>23</v>
@@ -612,7 +645,40 @@
         <v>20</v>
       </c>
     </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>26</v>
+      </c>
+      <c r="C6" t="s">
+        <v>27</v>
+      </c>
+      <c r="D6" t="s">
+        <v>23</v>
+      </c>
+      <c r="E6">
+        <v>50</v>
+      </c>
+      <c r="F6">
+        <v>50</v>
+      </c>
+      <c r="G6">
+        <v>50</v>
+      </c>
+      <c r="H6">
+        <v>50</v>
+      </c>
+      <c r="J6" t="s">
+        <v>28</v>
+      </c>
+      <c r="K6" t="s">
+        <v>20</v>
+      </c>
+    </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Módulo 'deletar encomenda': Ok, pequena correção no 'new_chart'
</commit_message>
<xml_diff>
--- a/dados.xlsx
+++ b/dados.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jeanc\Desktop\Projeto\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B8E8ACC-4BA8-4D6B-A63C-DD613937398E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31556C33-A685-455C-86C3-65E68B5BACCB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="20370" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="34">
   <si>
     <t>ID</t>
   </si>
@@ -55,77 +55,73 @@
     <t>Status</t>
   </si>
   <si>
-    <t>Daniel</t>
+    <t>Jean</t>
   </si>
   <si>
     <t>30/12/2021</t>
   </si>
   <si>
-    <t>08:00</t>
-  </si>
-  <si>
-    <t>muito chocolate</t>
+    <t>00:00</t>
+  </si>
+  <si>
+    <t>asdf</t>
   </si>
   <si>
     <t>Concluído</t>
   </si>
   <si>
-    <t>Jean</t>
-  </si>
-  <si>
-    <t>31/12/2021</t>
-  </si>
-  <si>
-    <t>20:00</t>
-  </si>
-  <si>
-    <t>bacon</t>
-  </si>
-  <si>
-    <t>Pendente</t>
-  </si>
-  <si>
-    <t>Selma</t>
-  </si>
-  <si>
-    <t>01/01/2022</t>
-  </si>
-  <si>
-    <t>00:00</t>
-  </si>
-  <si>
-    <t>joazinho</t>
-  </si>
-  <si>
-    <t>alimento</t>
-  </si>
-  <si>
-    <t>JEAN CARLOS</t>
-  </si>
-  <si>
-    <t>20/12/2022</t>
-  </si>
-  <si>
-    <t>TESTE
-TESTE
-TESTE
-TESTE
-TESTE
-TESE
-TESTE
-TESTE
-TESTE
-TEST
-TEST
-TES
-TE
-TEST
-TESTE
-ETSTE
-TETSS</t>
-  </si>
-  <si>
-    <t>01/01/2023</t>
+    <t>30/12/2022</t>
+  </si>
+  <si>
+    <t>00:01</t>
+  </si>
+  <si>
+    <t>30/12/2023</t>
+  </si>
+  <si>
+    <t>00:02</t>
+  </si>
+  <si>
+    <t>30/12/2024</t>
+  </si>
+  <si>
+    <t>00:03</t>
+  </si>
+  <si>
+    <t>30/12/2025</t>
+  </si>
+  <si>
+    <t>00:04</t>
+  </si>
+  <si>
+    <t>30/12/2026</t>
+  </si>
+  <si>
+    <t>00:05</t>
+  </si>
+  <si>
+    <t>30/12/2027</t>
+  </si>
+  <si>
+    <t>00:06</t>
+  </si>
+  <si>
+    <t>30/12/2028</t>
+  </si>
+  <si>
+    <t>00:07</t>
+  </si>
+  <si>
+    <t>30/12/2029</t>
+  </si>
+  <si>
+    <t>00:08</t>
+  </si>
+  <si>
+    <t>30/12/2030</t>
+  </si>
+  <si>
+    <t>00:09</t>
   </si>
 </sst>
 </file>
@@ -471,15 +467,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K6"/>
+  <dimension ref="A1:K11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="M9" sqref="M9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="18.42578125" customWidth="1"/>
+    <col min="3" max="3" width="11.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
@@ -531,19 +527,19 @@
         <v>13</v>
       </c>
       <c r="E2">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F2">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G2">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H2">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="I2">
-        <v>302.2</v>
+        <v>750</v>
       </c>
       <c r="J2" t="s">
         <v>14</v>
@@ -557,31 +553,34 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" t="s">
         <v>16</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>17</v>
       </c>
-      <c r="D3" t="s">
-        <v>18</v>
-      </c>
       <c r="E3">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F3">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G3">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H3">
-        <v>2</v>
+        <v>0</v>
+      </c>
+      <c r="I3">
+        <v>750</v>
       </c>
       <c r="J3" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="K3" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
@@ -589,19 +588,19 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>21</v>
+        <v>11</v>
       </c>
       <c r="C4" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="D4" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="E4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G4">
         <v>0</v>
@@ -609,8 +608,14 @@
       <c r="H4">
         <v>0</v>
       </c>
+      <c r="I4">
+        <v>750</v>
+      </c>
+      <c r="J4" t="s">
+        <v>14</v>
+      </c>
       <c r="K4" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
@@ -618,31 +623,34 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>24</v>
+        <v>11</v>
       </c>
       <c r="C5" t="s">
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="D5" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="E5">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="F5">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="G5">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="H5">
-        <v>20</v>
+        <v>0</v>
+      </c>
+      <c r="I5">
+        <v>750</v>
       </c>
       <c r="J5" t="s">
-        <v>25</v>
+        <v>14</v>
       </c>
       <c r="K5" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
@@ -650,31 +658,209 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>26</v>
+        <v>11</v>
       </c>
       <c r="C6" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="D6" t="s">
         <v>23</v>
       </c>
       <c r="E6">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="F6">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="G6">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="H6">
-        <v>50</v>
+        <v>0</v>
+      </c>
+      <c r="I6">
+        <v>750</v>
       </c>
       <c r="J6" t="s">
+        <v>14</v>
+      </c>
+      <c r="K6" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7" t="s">
+        <v>24</v>
+      </c>
+      <c r="D7" t="s">
+        <v>25</v>
+      </c>
+      <c r="E7">
+        <v>0</v>
+      </c>
+      <c r="F7">
+        <v>0</v>
+      </c>
+      <c r="G7">
+        <v>0</v>
+      </c>
+      <c r="H7">
+        <v>0</v>
+      </c>
+      <c r="I7">
+        <v>750</v>
+      </c>
+      <c r="J7" t="s">
+        <v>14</v>
+      </c>
+      <c r="K7" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>11</v>
+      </c>
+      <c r="C8" t="s">
+        <v>26</v>
+      </c>
+      <c r="D8" t="s">
+        <v>27</v>
+      </c>
+      <c r="E8">
+        <v>0</v>
+      </c>
+      <c r="F8">
+        <v>0</v>
+      </c>
+      <c r="G8">
+        <v>0</v>
+      </c>
+      <c r="H8">
+        <v>0</v>
+      </c>
+      <c r="I8">
+        <v>750</v>
+      </c>
+      <c r="J8" t="s">
+        <v>14</v>
+      </c>
+      <c r="K8" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>11</v>
+      </c>
+      <c r="C9" t="s">
         <v>28</v>
       </c>
-      <c r="K6" t="s">
-        <v>20</v>
+      <c r="D9" t="s">
+        <v>29</v>
+      </c>
+      <c r="E9">
+        <v>0</v>
+      </c>
+      <c r="F9">
+        <v>0</v>
+      </c>
+      <c r="G9">
+        <v>0</v>
+      </c>
+      <c r="H9">
+        <v>0</v>
+      </c>
+      <c r="I9">
+        <v>750</v>
+      </c>
+      <c r="J9" t="s">
+        <v>14</v>
+      </c>
+      <c r="K9" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>11</v>
+      </c>
+      <c r="C10" t="s">
+        <v>30</v>
+      </c>
+      <c r="D10" t="s">
+        <v>31</v>
+      </c>
+      <c r="E10">
+        <v>0</v>
+      </c>
+      <c r="F10">
+        <v>0</v>
+      </c>
+      <c r="G10">
+        <v>0</v>
+      </c>
+      <c r="H10">
+        <v>0</v>
+      </c>
+      <c r="I10">
+        <v>750</v>
+      </c>
+      <c r="J10" t="s">
+        <v>14</v>
+      </c>
+      <c r="K10" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
+        <v>11</v>
+      </c>
+      <c r="C11" t="s">
+        <v>32</v>
+      </c>
+      <c r="D11" t="s">
+        <v>33</v>
+      </c>
+      <c r="E11">
+        <v>0</v>
+      </c>
+      <c r="F11">
+        <v>0</v>
+      </c>
+      <c r="G11">
+        <v>0</v>
+      </c>
+      <c r="H11">
+        <v>0</v>
+      </c>
+      <c r="I11">
+        <v>750</v>
+      </c>
+      <c r="J11" t="s">
+        <v>14</v>
+      </c>
+      <c r="K11" t="s">
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
ATUALIZAÇÃO - LISTA VAZIA
</commit_message>
<xml_diff>
--- a/dados.xlsx
+++ b/dados.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K2"/>
+  <dimension ref="A1:K1"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="E15" sqref="E15"/>
@@ -481,44 +481,6 @@
         </is>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" t="n">
-        <v>1</v>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>Jean</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>02/05/2005</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>00:00</t>
-        </is>
-      </c>
-      <c r="E2" t="n">
-        <v>5</v>
-      </c>
-      <c r="F2" t="n">
-        <v>6</v>
-      </c>
-      <c r="G2" t="n">
-        <v>50</v>
-      </c>
-      <c r="H2" t="n">
-        <v>60</v>
-      </c>
-      <c r="J2" t="inlineStr"/>
-      <c r="K2" t="inlineStr">
-        <is>
-          <t>Pendente</t>
-        </is>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Primeiras verificações de entradas
</commit_message>
<xml_diff>
--- a/dados.xlsx
+++ b/dados.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K2"/>
+  <dimension ref="A1:K8"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="E15" sqref="E15"/>
@@ -524,6 +524,229 @@
         </is>
       </c>
     </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>JEan</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>02/05/2005</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>00:00</t>
+        </is>
+      </c>
+      <c r="E3" t="n">
+        <v>0</v>
+      </c>
+      <c r="F3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G3" t="n">
+        <v>0</v>
+      </c>
+      <c r="H3" t="n">
+        <v>0</v>
+      </c>
+      <c r="K3" t="inlineStr">
+        <is>
+          <t>Pendente</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Jean</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>32/13/20221</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>10:20</t>
+        </is>
+      </c>
+      <c r="E4" t="n">
+        <v>0</v>
+      </c>
+      <c r="F4" t="n">
+        <v>0</v>
+      </c>
+      <c r="G4" t="n">
+        <v>0</v>
+      </c>
+      <c r="H4" t="n">
+        <v>0</v>
+      </c>
+      <c r="K4" t="inlineStr">
+        <is>
+          <t>Pendente</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>4</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Jean</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>01/01/2021</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>10:33</t>
+        </is>
+      </c>
+      <c r="E5" t="n">
+        <v>0</v>
+      </c>
+      <c r="F5" t="n">
+        <v>0</v>
+      </c>
+      <c r="G5" t="n">
+        <v>0</v>
+      </c>
+      <c r="H5" t="n">
+        <v>0</v>
+      </c>
+      <c r="K5" t="inlineStr">
+        <is>
+          <t>Pendente</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>5</v>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>AFSDFS</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>12/13/2022</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>10:45</t>
+        </is>
+      </c>
+      <c r="E6" t="n">
+        <v>0</v>
+      </c>
+      <c r="F6" t="n">
+        <v>0</v>
+      </c>
+      <c r="G6" t="n">
+        <v>0</v>
+      </c>
+      <c r="H6" t="n">
+        <v>0</v>
+      </c>
+      <c r="K6" t="inlineStr">
+        <is>
+          <t>Pendente</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>6</v>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Jean</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>01/01/2022</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>23:52</t>
+        </is>
+      </c>
+      <c r="E7" t="n">
+        <v>1</v>
+      </c>
+      <c r="F7" t="n">
+        <v>0</v>
+      </c>
+      <c r="G7" t="n">
+        <v>0</v>
+      </c>
+      <c r="H7" t="n">
+        <v>0</v>
+      </c>
+      <c r="K7" t="inlineStr">
+        <is>
+          <t>Pendente</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>7</v>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Jean</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>31/01/2022</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>10:50</t>
+        </is>
+      </c>
+      <c r="E8" t="n">
+        <v>1</v>
+      </c>
+      <c r="F8" t="n">
+        <v>0</v>
+      </c>
+      <c r="G8" t="n">
+        <v>10</v>
+      </c>
+      <c r="H8" t="n">
+        <v>15</v>
+      </c>
+      <c r="J8" t="inlineStr"/>
+      <c r="K8" t="inlineStr">
+        <is>
+          <t>Pendente</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
NOVA ENCOMENDA: Requisitos funcionais implementados
</commit_message>
<xml_diff>
--- a/dados.xlsx
+++ b/dados.xlsx
@@ -45,9 +45,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -413,10 +412,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K8"/>
+  <dimension ref="A1:K1"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+      <selection activeCell="K7" sqref="A5:K7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
@@ -481,272 +480,6 @@
         </is>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" t="n">
-        <v>1</v>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>Jean Carlos Rodrigues Sousa</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>01/01/2022</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>00:00</t>
-        </is>
-      </c>
-      <c r="E2" t="n">
-        <v>1</v>
-      </c>
-      <c r="F2" t="n">
-        <v>2</v>
-      </c>
-      <c r="G2" t="n">
-        <v>3</v>
-      </c>
-      <c r="H2" t="n">
-        <v>4</v>
-      </c>
-      <c r="J2" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> teste
-sfasdfasdfasdf</t>
-        </is>
-      </c>
-      <c r="K2" t="inlineStr">
-        <is>
-          <t>Pendente</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="n">
-        <v>2</v>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>JEan</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>02/05/2005</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>00:00</t>
-        </is>
-      </c>
-      <c r="E3" t="n">
-        <v>0</v>
-      </c>
-      <c r="F3" t="n">
-        <v>0</v>
-      </c>
-      <c r="G3" t="n">
-        <v>0</v>
-      </c>
-      <c r="H3" t="n">
-        <v>0</v>
-      </c>
-      <c r="K3" t="inlineStr">
-        <is>
-          <t>Pendente</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="n">
-        <v>3</v>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>Jean</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>32/13/20221</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>10:20</t>
-        </is>
-      </c>
-      <c r="E4" t="n">
-        <v>0</v>
-      </c>
-      <c r="F4" t="n">
-        <v>0</v>
-      </c>
-      <c r="G4" t="n">
-        <v>0</v>
-      </c>
-      <c r="H4" t="n">
-        <v>0</v>
-      </c>
-      <c r="K4" t="inlineStr">
-        <is>
-          <t>Pendente</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="n">
-        <v>4</v>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>Jean</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>01/01/2021</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>10:33</t>
-        </is>
-      </c>
-      <c r="E5" t="n">
-        <v>0</v>
-      </c>
-      <c r="F5" t="n">
-        <v>0</v>
-      </c>
-      <c r="G5" t="n">
-        <v>0</v>
-      </c>
-      <c r="H5" t="n">
-        <v>0</v>
-      </c>
-      <c r="K5" t="inlineStr">
-        <is>
-          <t>Pendente</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="n">
-        <v>5</v>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>AFSDFS</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>12/13/2022</t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>10:45</t>
-        </is>
-      </c>
-      <c r="E6" t="n">
-        <v>0</v>
-      </c>
-      <c r="F6" t="n">
-        <v>0</v>
-      </c>
-      <c r="G6" t="n">
-        <v>0</v>
-      </c>
-      <c r="H6" t="n">
-        <v>0</v>
-      </c>
-      <c r="K6" t="inlineStr">
-        <is>
-          <t>Pendente</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="n">
-        <v>6</v>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>Jean</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>01/01/2022</t>
-        </is>
-      </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>23:52</t>
-        </is>
-      </c>
-      <c r="E7" t="n">
-        <v>1</v>
-      </c>
-      <c r="F7" t="n">
-        <v>0</v>
-      </c>
-      <c r="G7" t="n">
-        <v>0</v>
-      </c>
-      <c r="H7" t="n">
-        <v>0</v>
-      </c>
-      <c r="K7" t="inlineStr">
-        <is>
-          <t>Pendente</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="n">
-        <v>7</v>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>Jean</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>31/01/2022</t>
-        </is>
-      </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>10:50</t>
-        </is>
-      </c>
-      <c r="E8" t="n">
-        <v>1</v>
-      </c>
-      <c r="F8" t="n">
-        <v>0</v>
-      </c>
-      <c r="G8" t="n">
-        <v>10</v>
-      </c>
-      <c r="H8" t="n">
-        <v>15</v>
-      </c>
-      <c r="J8" t="inlineStr"/>
-      <c r="K8" t="inlineStr">
-        <is>
-          <t>Pendente</t>
-        </is>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Otimização da edição de encomenda
</commit_message>
<xml_diff>
--- a/dados.xlsx
+++ b/dados.xlsx
@@ -412,7 +412,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K1"/>
+  <dimension ref="A1:K2"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="K7" sqref="A5:K7"/>
@@ -480,6 +480,44 @@
         </is>
       </c>
     </row>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Carlos</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>02/05/2005</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>00:00</t>
+        </is>
+      </c>
+      <c r="E2" t="n">
+        <v>10</v>
+      </c>
+      <c r="F2" t="n">
+        <v>20</v>
+      </c>
+      <c r="G2" t="n">
+        <v>30</v>
+      </c>
+      <c r="H2" t="n">
+        <v>40</v>
+      </c>
+      <c r="J2" t="inlineStr"/>
+      <c r="K2" t="inlineStr">
+        <is>
+          <t>Pendente</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Alteração no método de listagem para se tornar mais suave
</commit_message>
<xml_diff>
--- a/dados.xlsx
+++ b/dados.xlsx
@@ -412,7 +412,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K2"/>
+  <dimension ref="A1:K1"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="K7" sqref="A5:K7"/>
@@ -480,44 +480,6 @@
         </is>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" t="n">
-        <v>1</v>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>Carlos</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>02/05/2005</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>00:00</t>
-        </is>
-      </c>
-      <c r="E2" t="n">
-        <v>10</v>
-      </c>
-      <c r="F2" t="n">
-        <v>20</v>
-      </c>
-      <c r="G2" t="n">
-        <v>30</v>
-      </c>
-      <c r="H2" t="n">
-        <v>40</v>
-      </c>
-      <c r="J2" t="inlineStr"/>
-      <c r="K2" t="inlineStr">
-        <is>
-          <t>Pendente</t>
-        </is>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Filtragem de data e hora completa
</commit_message>
<xml_diff>
--- a/dados.xlsx
+++ b/dados.xlsx
@@ -529,7 +529,7 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>02/12/2022</t>
+          <t>20/01/2023</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
@@ -538,16 +538,16 @@
         </is>
       </c>
       <c r="E3" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="F3" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="G3" t="n">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="H3" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="K3" t="inlineStr">
         <is>
@@ -566,7 +566,7 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>20/01/2023</t>
+          <t>02/03/2021</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
@@ -575,20 +575,23 @@
         </is>
       </c>
       <c r="E4" t="n">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="F4" t="n">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="G4" t="n">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="H4" t="n">
-        <v>0</v>
+        <v>50</v>
+      </c>
+      <c r="I4" t="n">
+        <v>25805</v>
       </c>
       <c r="K4" t="inlineStr">
         <is>
-          <t>Pendente</t>
+          <t>Concluído</t>
         </is>
       </c>
     </row>
@@ -598,12 +601,12 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Teste</t>
+          <t>Jean Carlos</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>02/05/2005</t>
+          <t>03/01/2022</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
@@ -612,7 +615,7 @@
         </is>
       </c>
       <c r="E5" t="n">
-        <v>50</v>
+        <v>1</v>
       </c>
       <c r="F5" t="n">
         <v>0</v>
@@ -640,32 +643,30 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>02/03/2021</t>
+          <t>03/01/2022</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>00:00</t>
+          <t>10:30</t>
         </is>
       </c>
       <c r="E6" t="n">
-        <v>50</v>
+        <v>1</v>
       </c>
       <c r="F6" t="n">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="G6" t="n">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="H6" t="n">
-        <v>50</v>
-      </c>
-      <c r="I6" t="n">
-        <v>25805</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="J6" t="inlineStr"/>
       <c r="K6" t="inlineStr">
         <is>
-          <t>Concluído</t>
+          <t>Pendente</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
TODOS OS ERROS TRATADOS
</commit_message>
<xml_diff>
--- a/dados.xlsx
+++ b/dados.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K6"/>
+  <dimension ref="A1:K7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -529,16 +529,16 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>20/01/2023</t>
+          <t>03/01/2022</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>00:00</t>
+          <t>10:00</t>
         </is>
       </c>
       <c r="E3" t="n">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="F3" t="n">
         <v>0</v>
@@ -549,6 +549,7 @@
       <c r="H3" t="n">
         <v>0</v>
       </c>
+      <c r="J3" t="inlineStr"/>
       <c r="K3" t="inlineStr">
         <is>
           <t>Pendente</t>
@@ -663,8 +664,44 @@
       <c r="H6" t="n">
         <v>0</v>
       </c>
-      <c r="J6" t="inlineStr"/>
       <c r="K6" t="inlineStr">
+        <is>
+          <t>Pendente</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>6</v>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Jean</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>02/01/2022</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>22:45</t>
+        </is>
+      </c>
+      <c r="E7" t="n">
+        <v>1</v>
+      </c>
+      <c r="F7" t="n">
+        <v>0</v>
+      </c>
+      <c r="G7" t="n">
+        <v>0</v>
+      </c>
+      <c r="H7" t="n">
+        <v>0</v>
+      </c>
+      <c r="K7" t="inlineStr">
         <is>
           <t>Pendente</t>
         </is>

</xml_diff>